<commit_message>
'foaie2' - duminică 20 februarie 2022, 15:48:43 +0200 alex T460
</commit_message>
<xml_diff>
--- a/foaie.xlsx
+++ b/foaie.xlsx
@@ -7,17 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="mai 1975" sheetId="1" r:id="rId1"/>
+    <sheet name="ianuarie 2022" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'mai 1975'!$A$1:$F$91</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'ianuarie 2022'!$A$1:$F$91</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -43,7 +43,7 @@
     <t>NPC</t>
   </si>
   <si>
-    <t>mai</t>
+    <t>ianuarie</t>
   </si>
   <si>
     <t>Alex Bora</t>
@@ -70,7 +70,7 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
-    <t>Cluj-Turda</t>
+    <t>Cluj-Cmp. Turzii</t>
   </si>
   <si>
     <t>Interes Serviciu</t>
@@ -82,10 +82,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
+    <t>Cluj-Zalau</t>
+  </si>
+  <si>
+    <t>Cluj-Apahida</t>
   </si>
   <si>
     <t>Cluj-Dej</t>
@@ -94,13 +94,7 @@
     <t>Cluj-Baia-Mare</t>
   </si>
   <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
-    <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
+    <t>Cluj-Bistrita</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -602,7 +596,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>1975</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -639,7 +633,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>7</v>
+        <v>89874</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -676,24 +670,36 @@
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="B19" s="4">
+        <v>152</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="4">
         <v>4</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="4">
+        <v>30</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4">
         <v>5</v>
       </c>
       <c r="B23" s="4">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>17</v>
@@ -707,13 +713,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="4">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -721,71 +727,71 @@
         <v>7</v>
       </c>
       <c r="B27" s="4">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4">
         <v>8</v>
       </c>
-      <c r="B29" s="4">
-        <v>152</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4">
         <v>9</v>
       </c>
-      <c r="B31" s="4">
-        <v>92</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4">
         <v>10</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="B33" s="4">
+        <v>30</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="4">
         <v>11</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+      <c r="B35" s="4">
+        <v>30</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="4">
         <v>12</v>
       </c>
       <c r="B37" s="4">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -793,13 +799,13 @@
         <v>13</v>
       </c>
       <c r="B39" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -820,58 +826,58 @@
       <c r="A43" s="4">
         <v>15</v>
       </c>
-      <c r="B43" s="4">
-        <v>30</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="4">
         <v>16</v>
       </c>
-      <c r="B45" s="4">
-        <v>92</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="4">
         <v>17</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="B47" s="4">
+        <v>30</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="4">
         <v>18</v>
       </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
+      <c r="B49" s="4">
+        <v>101</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="4">
         <v>19</v>
       </c>
       <c r="B51" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -879,13 +885,13 @@
         <v>20</v>
       </c>
       <c r="B53" s="4">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -906,29 +912,17 @@
       <c r="A57" s="4">
         <v>22</v>
       </c>
-      <c r="B57" s="4">
-        <v>356</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="4">
         <v>23</v>
       </c>
-      <c r="B59" s="4">
-        <v>30</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="4">
@@ -942,22 +936,28 @@
       <c r="A63" s="4">
         <v>25</v>
       </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
+      <c r="B63" s="4">
+        <v>30</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="4">
         <v>26</v>
       </c>
       <c r="B65" s="4">
-        <v>356</v>
+        <v>30</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -965,10 +965,10 @@
         <v>27</v>
       </c>
       <c r="B67" s="4">
-        <v>47</v>
+        <v>356</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>18</v>
@@ -979,10 +979,10 @@
         <v>28</v>
       </c>
       <c r="B69" s="4">
-        <v>356</v>
+        <v>257</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>18</v>
@@ -992,57 +992,51 @@
       <c r="A71" s="4">
         <v>29</v>
       </c>
-      <c r="B71" s="4">
-        <v>121</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="4">
         <v>30</v>
       </c>
-      <c r="B73" s="4">
-        <v>421</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="4">
         <v>31</v>
       </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
+      <c r="B75" s="4">
+        <v>356</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B76" s="5">
-        <v>3028</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B77" s="5">
-        <v>3035</v>
+        <v>91920</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -1056,7 +1050,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -1064,7 +1058,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -1072,7 +1066,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -1080,7 +1074,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -1094,7 +1088,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>

</xml_diff>